<commit_message>
refactor code and handle errors
</commit_message>
<xml_diff>
--- a/data_magento.xlsx
+++ b/data_magento.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>000001209</t>
+          <t>000001305</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>000001209</t>
+          <t>000001305</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>

<commit_message>
handle error link product
</commit_message>
<xml_diff>
--- a/data_magento.xlsx
+++ b/data_magento.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>Color</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -461,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -471,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>000001321</t>
+          <t>000001323</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -482,6 +487,11 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>Blue</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>09:46:04 2024-05-14</t>
         </is>
       </c>
     </row>
@@ -503,7 +513,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>000001321</t>
+          <t>000001323</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -514,6 +524,11 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>Blue</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>09:46:04 2024-05-14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor for go to page of the website
</commit_message>
<xml_diff>
--- a/data_magento.xlsx
+++ b/data_magento.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Proteus Fitness Jackshirt</t>
+          <t>Cassius Sparring Tank</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -471,17 +471,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$45.00</t>
+          <t>$18.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>000001323</t>
+          <t>000001486</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>XL</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -491,44 +491,599 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>09:46:04 2024-05-14</t>
+          <t>11:04:44 2024-05-15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Atlas Fitness Tank</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$18.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sinbad Fitness Tank</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$29.00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rocco Gym Tank</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$24.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Helios Endurance Tank</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$32.00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Primo Endurance Tank</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$29.00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Strike Endurance Tee</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$39.00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Logan HeatTec® Tee</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$24.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ryker LumaTech™ Tee (V-neck)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$28.00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Zoltan Gym Tee</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$29.00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Atomic Endurance Running Tee (Crew-Neck)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$29.00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Atomic Endurance Running Tee (V-neck)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$28.00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ryker LumaTech™ Tee (Crew-neck)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$32.00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Helios EverCool™ Tee</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$24.00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Proteus Fitness Jackshirt</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$45.00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>Kenobi Trail Jacket</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>$47.00</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>000001323</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Blue</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>09:46:04 2024-05-14</t>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Stark Fundamental Hoodie</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$42.00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>000001486</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>11:04:44 2024-05-15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
complete get all pages
</commit_message>
<xml_diff>
--- a/data_magento.xlsx
+++ b/data_magento.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -587,7 +587,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -735,7 +735,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -772,7 +772,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -898,7 +898,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>000001486</t>
+          <t>000001702</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>11:04:44 2024-05-15</t>
+          <t>10:31:47 2024-05-16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upgrade robot has a navigation all page and log out website
</commit_message>
<xml_diff>
--- a/data_magento.xlsx
+++ b/data_magento.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -772,7 +772,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -898,7 +898,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -994,7 +994,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>000001702</t>
+          <t>000002745</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>10:31:47 2024-05-16</t>
+          <t>23:05:19 2024-05-21</t>
         </is>
       </c>
     </row>

</xml_diff>